<commit_message>
feat: adicionar criação de banco de dados
</commit_message>
<xml_diff>
--- a/SpotifyClone-Non-NormalizedTable-fav-songs.xlsx
+++ b/SpotifyClone-Non-NormalizedTable-fav-songs.xlsx
@@ -444,7 +444,7 @@
     <col min="2" max="2" style="3" width="88.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -460,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -468,7 +468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -476,7 +476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -484,7 +484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -492,7 +492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -508,7 +508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>